<commit_message>
se modifica archivo excel
</commit_message>
<xml_diff>
--- a/clientes-kmeans.xlsx
+++ b/clientes-kmeans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documentos Willy\Ciencia_de_Datos_IA\2025\Trayecto_G\Trabajo2\Kmeans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{434AB358-597F-472E-BC36-A01CF5B88DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B29F98E-7DA7-4536-BA1F-9FE9A1D4E17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65A4316A-5845-4B96-884C-F1CBC2C00071}"/>
   </bookViews>
@@ -45,16 +45,16 @@
     <t>edad</t>
   </si>
   <si>
-    <t>ingresosSemanales(miles$)</t>
-  </si>
-  <si>
-    <t>puntaje(1-100)</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>ingresosSemanales</t>
+  </si>
+  <si>
+    <t>puntaje</t>
   </si>
 </sst>
 </file>
@@ -409,10 +409,14 @@
   <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.19921875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -425,10 +429,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -436,7 +440,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>19</v>
@@ -453,7 +457,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>21</v>
@@ -470,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -487,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>23</v>
@@ -504,7 +508,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>31</v>
@@ -521,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>22</v>
@@ -538,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>35</v>
@@ -555,7 +559,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>23</v>
@@ -572,7 +576,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>64</v>
@@ -589,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>30</v>
@@ -606,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>67</v>
@@ -623,7 +627,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>35</v>
@@ -640,7 +644,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>58</v>
@@ -657,7 +661,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>24</v>
@@ -674,7 +678,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>37</v>
@@ -691,7 +695,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>22</v>
@@ -708,7 +712,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>35</v>
@@ -725,7 +729,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>20</v>
@@ -742,7 +746,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>52</v>
@@ -759,7 +763,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>35</v>
@@ -776,7 +780,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>35</v>
@@ -793,7 +797,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>25</v>
@@ -810,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>46</v>
@@ -827,7 +831,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>31</v>
@@ -844,7 +848,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>54</v>
@@ -861,7 +865,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>29</v>
@@ -878,7 +882,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>45</v>
@@ -895,7 +899,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>35</v>
@@ -912,7 +916,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>40</v>
@@ -929,7 +933,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>23</v>
@@ -946,7 +950,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>60</v>
@@ -963,7 +967,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>21</v>
@@ -980,7 +984,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>53</v>
@@ -997,7 +1001,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>18</v>
@@ -1014,7 +1018,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>49</v>
@@ -1031,7 +1035,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>21</v>
@@ -1048,7 +1052,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>42</v>
@@ -1065,7 +1069,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>30</v>
@@ -1082,7 +1086,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>36</v>
@@ -1099,7 +1103,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>20</v>
@@ -1116,7 +1120,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>65</v>
@@ -1133,7 +1137,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>24</v>
@@ -1150,7 +1154,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>48</v>
@@ -1167,7 +1171,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>31</v>
@@ -1184,7 +1188,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>49</v>
@@ -1201,7 +1205,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>24</v>
@@ -1218,7 +1222,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>50</v>
@@ -1235,7 +1239,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>27</v>
@@ -1252,7 +1256,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C50">
         <v>29</v>
@@ -1269,7 +1273,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C51">
         <v>31</v>
@@ -1286,7 +1290,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C52">
         <v>49</v>
@@ -1303,7 +1307,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C53">
         <v>33</v>
@@ -1320,7 +1324,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C54">
         <v>31</v>
@@ -1337,7 +1341,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C55">
         <v>59</v>
@@ -1354,7 +1358,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C56">
         <v>50</v>
@@ -1371,7 +1375,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C57">
         <v>47</v>
@@ -1388,7 +1392,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C58">
         <v>51</v>
@@ -1405,7 +1409,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C59">
         <v>69</v>
@@ -1422,7 +1426,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C60">
         <v>27</v>
@@ -1439,7 +1443,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>53</v>
@@ -1456,7 +1460,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>70</v>
@@ -1473,7 +1477,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>19</v>
@@ -1490,7 +1494,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C64">
         <v>67</v>
@@ -1507,7 +1511,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>54</v>
@@ -1524,7 +1528,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C66">
         <v>63</v>
@@ -1541,7 +1545,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C67">
         <v>18</v>
@@ -1558,7 +1562,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C68">
         <v>43</v>
@@ -1575,7 +1579,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -1592,7 +1596,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C70">
         <v>19</v>
@@ -1609,7 +1613,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C71">
         <v>32</v>
@@ -1626,7 +1630,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C72">
         <v>70</v>
@@ -1643,7 +1647,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C73">
         <v>47</v>
@@ -1660,7 +1664,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C74">
         <v>60</v>
@@ -1677,7 +1681,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C75">
         <v>60</v>
@@ -1694,7 +1698,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C76">
         <v>59</v>
@@ -1711,7 +1715,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C77">
         <v>26</v>
@@ -1728,7 +1732,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C78">
         <v>45</v>
@@ -1745,7 +1749,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C79">
         <v>40</v>
@@ -1762,7 +1766,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C80">
         <v>23</v>
@@ -1779,7 +1783,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C81">
         <v>49</v>
@@ -1796,7 +1800,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C82">
         <v>57</v>
@@ -1813,7 +1817,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C83">
         <v>38</v>
@@ -1830,7 +1834,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C84">
         <v>67</v>
@@ -1847,7 +1851,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C85">
         <v>46</v>
@@ -1864,7 +1868,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C86">
         <v>21</v>
@@ -1881,7 +1885,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C87">
         <v>48</v>
@@ -1898,7 +1902,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C88">
         <v>55</v>
@@ -1915,7 +1919,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>22</v>
@@ -1932,7 +1936,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C90">
         <v>34</v>
@@ -1949,7 +1953,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C91">
         <v>50</v>
@@ -1966,7 +1970,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C92">
         <v>68</v>
@@ -1983,7 +1987,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C93">
         <v>18</v>
@@ -2000,7 +2004,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C94">
         <v>48</v>
@@ -2017,7 +2021,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C95">
         <v>40</v>
@@ -2034,7 +2038,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C96">
         <v>32</v>
@@ -2051,7 +2055,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C97">
         <v>24</v>
@@ -2068,7 +2072,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C98">
         <v>47</v>
@@ -2085,7 +2089,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C99">
         <v>27</v>
@@ -2102,7 +2106,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C100">
         <v>48</v>
@@ -2119,7 +2123,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C101">
         <v>20</v>
@@ -2136,7 +2140,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C102">
         <v>23</v>
@@ -2153,7 +2157,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C103">
         <v>49</v>
@@ -2170,7 +2174,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C104">
         <v>67</v>
@@ -2187,7 +2191,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C105">
         <v>26</v>
@@ -2204,7 +2208,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C106">
         <v>49</v>
@@ -2221,7 +2225,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C107">
         <v>21</v>
@@ -2238,7 +2242,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C108">
         <v>66</v>
@@ -2255,7 +2259,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C109">
         <v>54</v>
@@ -2272,7 +2276,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C110">
         <v>68</v>
@@ -2289,7 +2293,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C111">
         <v>66</v>
@@ -2306,7 +2310,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C112">
         <v>65</v>
@@ -2323,7 +2327,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C113">
         <v>19</v>
@@ -2340,7 +2344,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C114">
         <v>38</v>
@@ -2357,7 +2361,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C115">
         <v>19</v>
@@ -2374,7 +2378,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C116">
         <v>18</v>
@@ -2391,7 +2395,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C117">
         <v>19</v>
@@ -2408,7 +2412,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C118">
         <v>63</v>
@@ -2425,7 +2429,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C119">
         <v>49</v>
@@ -2442,7 +2446,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C120">
         <v>51</v>
@@ -2459,7 +2463,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C121">
         <v>50</v>
@@ -2476,7 +2480,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C122">
         <v>27</v>
@@ -2493,7 +2497,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C123">
         <v>38</v>
@@ -2510,7 +2514,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C124">
         <v>40</v>
@@ -2527,7 +2531,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C125">
         <v>39</v>
@@ -2544,7 +2548,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C126">
         <v>23</v>
@@ -2561,7 +2565,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C127">
         <v>31</v>
@@ -2578,7 +2582,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C128">
         <v>43</v>
@@ -2595,7 +2599,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C129">
         <v>40</v>
@@ -2612,7 +2616,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C130">
         <v>59</v>
@@ -2629,7 +2633,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C131">
         <v>38</v>
@@ -2646,7 +2650,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C132">
         <v>47</v>
@@ -2663,7 +2667,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C133">
         <v>39</v>
@@ -2680,7 +2684,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C134">
         <v>25</v>
@@ -2697,7 +2701,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C135">
         <v>31</v>
@@ -2714,7 +2718,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C136">
         <v>20</v>
@@ -2731,7 +2735,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C137">
         <v>29</v>
@@ -2748,7 +2752,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C138">
         <v>44</v>
@@ -2765,7 +2769,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C139">
         <v>32</v>
@@ -2782,7 +2786,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C140">
         <v>19</v>
@@ -2799,7 +2803,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C141">
         <v>35</v>
@@ -2816,7 +2820,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C142">
         <v>57</v>
@@ -2833,7 +2837,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C143">
         <v>32</v>
@@ -2850,7 +2854,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C144">
         <v>28</v>
@@ -2867,7 +2871,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C145">
         <v>32</v>
@@ -2884,7 +2888,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C146">
         <v>25</v>
@@ -2901,7 +2905,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C147">
         <v>28</v>
@@ -2918,7 +2922,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C148">
         <v>48</v>
@@ -2935,7 +2939,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C149">
         <v>32</v>
@@ -2952,7 +2956,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C150">
         <v>34</v>
@@ -2969,7 +2973,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C151">
         <v>34</v>
@@ -2986,7 +2990,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C152">
         <v>43</v>
@@ -3003,7 +3007,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C153">
         <v>39</v>
@@ -3020,7 +3024,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C154">
         <v>44</v>
@@ -3037,7 +3041,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C155">
         <v>38</v>
@@ -3054,7 +3058,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C156">
         <v>47</v>
@@ -3071,7 +3075,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C157">
         <v>27</v>
@@ -3088,7 +3092,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C158">
         <v>37</v>
@@ -3105,7 +3109,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C159">
         <v>30</v>
@@ -3122,7 +3126,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C160">
         <v>34</v>
@@ -3139,7 +3143,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C161">
         <v>30</v>
@@ -3156,7 +3160,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C162">
         <v>56</v>
@@ -3173,7 +3177,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C163">
         <v>29</v>
@@ -3190,7 +3194,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C164">
         <v>19</v>
@@ -3207,7 +3211,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C165">
         <v>31</v>
@@ -3224,7 +3228,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C166">
         <v>50</v>
@@ -3241,7 +3245,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C167">
         <v>36</v>
@@ -3258,7 +3262,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C168">
         <v>42</v>
@@ -3275,7 +3279,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C169">
         <v>33</v>
@@ -3292,7 +3296,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C170">
         <v>36</v>
@@ -3309,7 +3313,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C171">
         <v>32</v>
@@ -3326,7 +3330,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C172">
         <v>40</v>
@@ -3343,7 +3347,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C173">
         <v>28</v>
@@ -3360,7 +3364,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C174">
         <v>36</v>
@@ -3377,7 +3381,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C175">
         <v>36</v>
@@ -3394,7 +3398,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C176">
         <v>52</v>
@@ -3411,7 +3415,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C177">
         <v>30</v>
@@ -3428,7 +3432,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C178">
         <v>58</v>
@@ -3445,7 +3449,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C179">
         <v>27</v>
@@ -3462,7 +3466,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C180">
         <v>59</v>
@@ -3479,7 +3483,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C181">
         <v>35</v>
@@ -3496,7 +3500,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C182">
         <v>37</v>
@@ -3513,7 +3517,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C183">
         <v>32</v>
@@ -3530,7 +3534,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C184">
         <v>46</v>
@@ -3547,7 +3551,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C185">
         <v>29</v>
@@ -3564,7 +3568,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C186">
         <v>41</v>
@@ -3581,7 +3585,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C187">
         <v>30</v>
@@ -3598,7 +3602,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C188">
         <v>54</v>
@@ -3615,7 +3619,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C189">
         <v>28</v>
@@ -3632,7 +3636,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C190">
         <v>41</v>
@@ -3649,7 +3653,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C191">
         <v>36</v>
@@ -3666,7 +3670,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C192">
         <v>34</v>
@@ -3683,7 +3687,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C193">
         <v>32</v>
@@ -3700,7 +3704,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C194">
         <v>33</v>
@@ -3717,7 +3721,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C195">
         <v>38</v>
@@ -3734,7 +3738,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C196">
         <v>47</v>
@@ -3751,7 +3755,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C197">
         <v>35</v>
@@ -3768,7 +3772,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C198">
         <v>45</v>
@@ -3785,7 +3789,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C199">
         <v>32</v>
@@ -3802,7 +3806,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C200">
         <v>32</v>
@@ -3819,7 +3823,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C201">
         <v>30</v>

</xml_diff>

<commit_message>
Actualizo todos los archivos del proyecto
</commit_message>
<xml_diff>
--- a/clientes-kmeans.xlsx
+++ b/clientes-kmeans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documentos Willy\Ciencia_de_Datos_IA\2025\Trayecto_G\Trabajo2\Kmeans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B29F98E-7DA7-4536-BA1F-9FE9A1D4E17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5E481F-E1E8-4142-B5D6-F4DB68A12767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65A4316A-5845-4B96-884C-F1CBC2C00071}"/>
   </bookViews>
@@ -61,6 +61,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -90,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,13 +412,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A124DC84-9168-4E31-AB85-D334AFE8A5DD}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.19921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -428,7 +432,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
@@ -445,7 +449,7 @@
       <c r="C2">
         <v>19</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>15</v>
       </c>
       <c r="E2">
@@ -462,7 +466,7 @@
       <c r="C3">
         <v>21</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>15</v>
       </c>
       <c r="E3">
@@ -479,7 +483,7 @@
       <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>16</v>
       </c>
       <c r="E4">
@@ -496,7 +500,7 @@
       <c r="C5">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>16</v>
       </c>
       <c r="E5">
@@ -513,7 +517,7 @@
       <c r="C6">
         <v>31</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>17</v>
       </c>
       <c r="E6">
@@ -530,7 +534,7 @@
       <c r="C7">
         <v>22</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>17</v>
       </c>
       <c r="E7">
@@ -547,7 +551,7 @@
       <c r="C8">
         <v>35</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>18</v>
       </c>
       <c r="E8">
@@ -564,7 +568,7 @@
       <c r="C9">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>18</v>
       </c>
       <c r="E9">
@@ -581,7 +585,7 @@
       <c r="C10">
         <v>64</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>19</v>
       </c>
       <c r="E10">
@@ -598,7 +602,7 @@
       <c r="C11">
         <v>30</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>19</v>
       </c>
       <c r="E11">
@@ -615,7 +619,7 @@
       <c r="C12">
         <v>67</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>19</v>
       </c>
       <c r="E12">
@@ -632,7 +636,7 @@
       <c r="C13">
         <v>35</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>19</v>
       </c>
       <c r="E13">
@@ -649,7 +653,7 @@
       <c r="C14">
         <v>58</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>20</v>
       </c>
       <c r="E14">
@@ -666,7 +670,7 @@
       <c r="C15">
         <v>24</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>20</v>
       </c>
       <c r="E15">
@@ -683,7 +687,7 @@
       <c r="C16">
         <v>37</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>20</v>
       </c>
       <c r="E16">
@@ -700,7 +704,7 @@
       <c r="C17">
         <v>22</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>20</v>
       </c>
       <c r="E17">
@@ -717,7 +721,7 @@
       <c r="C18">
         <v>35</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>21</v>
       </c>
       <c r="E18">
@@ -734,7 +738,7 @@
       <c r="C19">
         <v>20</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>21</v>
       </c>
       <c r="E19">
@@ -751,7 +755,7 @@
       <c r="C20">
         <v>52</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>23</v>
       </c>
       <c r="E20">
@@ -768,7 +772,7 @@
       <c r="C21">
         <v>35</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>23</v>
       </c>
       <c r="E21">
@@ -785,7 +789,7 @@
       <c r="C22">
         <v>35</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>24</v>
       </c>
       <c r="E22">
@@ -802,7 +806,7 @@
       <c r="C23">
         <v>25</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>24</v>
       </c>
       <c r="E23">
@@ -819,7 +823,7 @@
       <c r="C24">
         <v>46</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>25</v>
       </c>
       <c r="E24">
@@ -836,7 +840,7 @@
       <c r="C25">
         <v>31</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>25</v>
       </c>
       <c r="E25">
@@ -853,7 +857,7 @@
       <c r="C26">
         <v>54</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>28</v>
       </c>
       <c r="E26">
@@ -870,7 +874,7 @@
       <c r="C27">
         <v>29</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>28</v>
       </c>
       <c r="E27">
@@ -887,7 +891,7 @@
       <c r="C28">
         <v>45</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>28</v>
       </c>
       <c r="E28">
@@ -904,7 +908,7 @@
       <c r="C29">
         <v>35</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>28</v>
       </c>
       <c r="E29">
@@ -921,7 +925,7 @@
       <c r="C30">
         <v>40</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>29</v>
       </c>
       <c r="E30">
@@ -938,7 +942,7 @@
       <c r="C31">
         <v>23</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>29</v>
       </c>
       <c r="E31">
@@ -955,7 +959,7 @@
       <c r="C32">
         <v>60</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>30</v>
       </c>
       <c r="E32">
@@ -972,7 +976,7 @@
       <c r="C33">
         <v>21</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>30</v>
       </c>
       <c r="E33">
@@ -989,7 +993,7 @@
       <c r="C34">
         <v>53</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>33</v>
       </c>
       <c r="E34">
@@ -1006,7 +1010,7 @@
       <c r="C35">
         <v>18</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>33</v>
       </c>
       <c r="E35">
@@ -1023,7 +1027,7 @@
       <c r="C36">
         <v>49</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>33</v>
       </c>
       <c r="E36">
@@ -1040,7 +1044,7 @@
       <c r="C37">
         <v>21</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>33</v>
       </c>
       <c r="E37">
@@ -1057,7 +1061,7 @@
       <c r="C38">
         <v>42</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>34</v>
       </c>
       <c r="E38">
@@ -1074,7 +1078,7 @@
       <c r="C39">
         <v>30</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>34</v>
       </c>
       <c r="E39">
@@ -1091,7 +1095,7 @@
       <c r="C40">
         <v>36</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>37</v>
       </c>
       <c r="E40">
@@ -1108,7 +1112,7 @@
       <c r="C41">
         <v>20</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>37</v>
       </c>
       <c r="E41">
@@ -1125,7 +1129,7 @@
       <c r="C42">
         <v>65</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>38</v>
       </c>
       <c r="E42">
@@ -1142,7 +1146,7 @@
       <c r="C43">
         <v>24</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>38</v>
       </c>
       <c r="E43">
@@ -1159,7 +1163,7 @@
       <c r="C44">
         <v>48</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>39</v>
       </c>
       <c r="E44">
@@ -1176,7 +1180,7 @@
       <c r="C45">
         <v>31</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>39</v>
       </c>
       <c r="E45">
@@ -1193,7 +1197,7 @@
       <c r="C46">
         <v>49</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>39</v>
       </c>
       <c r="E46">
@@ -1210,7 +1214,7 @@
       <c r="C47">
         <v>24</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>39</v>
       </c>
       <c r="E47">
@@ -1227,7 +1231,7 @@
       <c r="C48">
         <v>50</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>40</v>
       </c>
       <c r="E48">
@@ -1244,7 +1248,7 @@
       <c r="C49">
         <v>27</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>40</v>
       </c>
       <c r="E49">
@@ -1261,7 +1265,7 @@
       <c r="C50">
         <v>29</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>40</v>
       </c>
       <c r="E50">
@@ -1278,7 +1282,7 @@
       <c r="C51">
         <v>31</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>40</v>
       </c>
       <c r="E51">
@@ -1295,7 +1299,7 @@
       <c r="C52">
         <v>49</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>42</v>
       </c>
       <c r="E52">
@@ -1312,7 +1316,7 @@
       <c r="C53">
         <v>33</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>42</v>
       </c>
       <c r="E53">
@@ -1329,7 +1333,7 @@
       <c r="C54">
         <v>31</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>43</v>
       </c>
       <c r="E54">
@@ -1346,7 +1350,7 @@
       <c r="C55">
         <v>59</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>43</v>
       </c>
       <c r="E55">
@@ -1363,7 +1367,7 @@
       <c r="C56">
         <v>50</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>43</v>
       </c>
       <c r="E56">
@@ -1380,7 +1384,7 @@
       <c r="C57">
         <v>47</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>43</v>
       </c>
       <c r="E57">
@@ -1397,7 +1401,7 @@
       <c r="C58">
         <v>51</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>44</v>
       </c>
       <c r="E58">
@@ -1414,7 +1418,7 @@
       <c r="C59">
         <v>69</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>44</v>
       </c>
       <c r="E59">
@@ -1431,7 +1435,7 @@
       <c r="C60">
         <v>27</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="1">
         <v>46</v>
       </c>
       <c r="E60">
@@ -1448,7 +1452,7 @@
       <c r="C61">
         <v>53</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>46</v>
       </c>
       <c r="E61">
@@ -1465,7 +1469,7 @@
       <c r="C62">
         <v>70</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
         <v>46</v>
       </c>
       <c r="E62">
@@ -1482,7 +1486,7 @@
       <c r="C63">
         <v>19</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>46</v>
       </c>
       <c r="E63">
@@ -1499,7 +1503,7 @@
       <c r="C64">
         <v>67</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
         <v>47</v>
       </c>
       <c r="E64">
@@ -1516,7 +1520,7 @@
       <c r="C65">
         <v>54</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="1">
         <v>47</v>
       </c>
       <c r="E65">
@@ -1533,7 +1537,7 @@
       <c r="C66">
         <v>63</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>48</v>
       </c>
       <c r="E66">
@@ -1550,7 +1554,7 @@
       <c r="C67">
         <v>18</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="1">
         <v>48</v>
       </c>
       <c r="E67">
@@ -1567,7 +1571,7 @@
       <c r="C68">
         <v>43</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>48</v>
       </c>
       <c r="E68">
@@ -1584,7 +1588,7 @@
       <c r="C69">
         <v>68</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="1">
         <v>48</v>
       </c>
       <c r="E69">
@@ -1601,7 +1605,7 @@
       <c r="C70">
         <v>19</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>48</v>
       </c>
       <c r="E70">
@@ -1618,7 +1622,7 @@
       <c r="C71">
         <v>32</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>48</v>
       </c>
       <c r="E71">
@@ -1635,7 +1639,7 @@
       <c r="C72">
         <v>70</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
         <v>49</v>
       </c>
       <c r="E72">
@@ -1652,7 +1656,7 @@
       <c r="C73">
         <v>47</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="1">
         <v>49</v>
       </c>
       <c r="E73">
@@ -1669,7 +1673,7 @@
       <c r="C74">
         <v>60</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>50</v>
       </c>
       <c r="E74">
@@ -1686,7 +1690,7 @@
       <c r="C75">
         <v>60</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="1">
         <v>50</v>
       </c>
       <c r="E75">
@@ -1703,7 +1707,7 @@
       <c r="C76">
         <v>59</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="1">
         <v>54</v>
       </c>
       <c r="E76">
@@ -1720,7 +1724,7 @@
       <c r="C77">
         <v>26</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="1">
         <v>54</v>
       </c>
       <c r="E77">
@@ -1737,7 +1741,7 @@
       <c r="C78">
         <v>45</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="1">
         <v>54</v>
       </c>
       <c r="E78">
@@ -1754,7 +1758,7 @@
       <c r="C79">
         <v>40</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="1">
         <v>54</v>
       </c>
       <c r="E79">
@@ -1771,7 +1775,7 @@
       <c r="C80">
         <v>23</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>54</v>
       </c>
       <c r="E80">
@@ -1788,7 +1792,7 @@
       <c r="C81">
         <v>49</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="1">
         <v>54</v>
       </c>
       <c r="E81">
@@ -1805,7 +1809,7 @@
       <c r="C82">
         <v>57</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="1">
         <v>54</v>
       </c>
       <c r="E82">
@@ -1822,7 +1826,7 @@
       <c r="C83">
         <v>38</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
         <v>54</v>
       </c>
       <c r="E83">
@@ -1839,7 +1843,7 @@
       <c r="C84">
         <v>67</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>54</v>
       </c>
       <c r="E84">
@@ -1856,7 +1860,7 @@
       <c r="C85">
         <v>46</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="1">
         <v>54</v>
       </c>
       <c r="E85">
@@ -1873,7 +1877,7 @@
       <c r="C86">
         <v>21</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>54</v>
       </c>
       <c r="E86">
@@ -1890,7 +1894,7 @@
       <c r="C87">
         <v>48</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="1">
         <v>54</v>
       </c>
       <c r="E87">
@@ -1907,7 +1911,7 @@
       <c r="C88">
         <v>55</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
         <v>57</v>
       </c>
       <c r="E88">
@@ -1924,7 +1928,7 @@
       <c r="C89">
         <v>22</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
         <v>57</v>
       </c>
       <c r="E89">
@@ -1941,7 +1945,7 @@
       <c r="C90">
         <v>34</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="1">
         <v>58</v>
       </c>
       <c r="E90">
@@ -1958,7 +1962,7 @@
       <c r="C91">
         <v>50</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="1">
         <v>58</v>
       </c>
       <c r="E91">
@@ -1975,7 +1979,7 @@
       <c r="C92">
         <v>68</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="1">
         <v>59</v>
       </c>
       <c r="E92">
@@ -1992,7 +1996,7 @@
       <c r="C93">
         <v>18</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="1">
         <v>59</v>
       </c>
       <c r="E93">
@@ -2009,7 +2013,7 @@
       <c r="C94">
         <v>48</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="1">
         <v>60</v>
       </c>
       <c r="E94">
@@ -2026,7 +2030,7 @@
       <c r="C95">
         <v>40</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="1">
         <v>60</v>
       </c>
       <c r="E95">
@@ -2043,7 +2047,7 @@
       <c r="C96">
         <v>32</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="1">
         <v>60</v>
       </c>
       <c r="E96">
@@ -2060,7 +2064,7 @@
       <c r="C97">
         <v>24</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="1">
         <v>60</v>
       </c>
       <c r="E97">
@@ -2077,7 +2081,7 @@
       <c r="C98">
         <v>47</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="1">
         <v>60</v>
       </c>
       <c r="E98">
@@ -2094,7 +2098,7 @@
       <c r="C99">
         <v>27</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="1">
         <v>60</v>
       </c>
       <c r="E99">
@@ -2111,7 +2115,7 @@
       <c r="C100">
         <v>48</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="1">
         <v>61</v>
       </c>
       <c r="E100">
@@ -2128,7 +2132,7 @@
       <c r="C101">
         <v>20</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="1">
         <v>61</v>
       </c>
       <c r="E101">
@@ -2145,7 +2149,7 @@
       <c r="C102">
         <v>23</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="1">
         <v>62</v>
       </c>
       <c r="E102">
@@ -2162,7 +2166,7 @@
       <c r="C103">
         <v>49</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="1">
         <v>62</v>
       </c>
       <c r="E103">
@@ -2179,7 +2183,7 @@
       <c r="C104">
         <v>67</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="1">
         <v>62</v>
       </c>
       <c r="E104">
@@ -2196,7 +2200,7 @@
       <c r="C105">
         <v>26</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="1">
         <v>62</v>
       </c>
       <c r="E105">
@@ -2213,7 +2217,7 @@
       <c r="C106">
         <v>49</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="1">
         <v>62</v>
       </c>
       <c r="E106">
@@ -2230,7 +2234,7 @@
       <c r="C107">
         <v>21</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="1">
         <v>62</v>
       </c>
       <c r="E107">
@@ -2247,7 +2251,7 @@
       <c r="C108">
         <v>66</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="1">
         <v>63</v>
       </c>
       <c r="E108">
@@ -2264,7 +2268,7 @@
       <c r="C109">
         <v>54</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="1">
         <v>63</v>
       </c>
       <c r="E109">
@@ -2281,7 +2285,7 @@
       <c r="C110">
         <v>68</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="1">
         <v>63</v>
       </c>
       <c r="E110">
@@ -2298,7 +2302,7 @@
       <c r="C111">
         <v>66</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="1">
         <v>63</v>
       </c>
       <c r="E111">
@@ -2315,7 +2319,7 @@
       <c r="C112">
         <v>65</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="1">
         <v>63</v>
       </c>
       <c r="E112">
@@ -2332,7 +2336,7 @@
       <c r="C113">
         <v>19</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="1">
         <v>63</v>
       </c>
       <c r="E113">
@@ -2349,7 +2353,7 @@
       <c r="C114">
         <v>38</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="1">
         <v>64</v>
       </c>
       <c r="E114">
@@ -2366,7 +2370,7 @@
       <c r="C115">
         <v>19</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="1">
         <v>64</v>
       </c>
       <c r="E115">
@@ -2383,7 +2387,7 @@
       <c r="C116">
         <v>18</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="1">
         <v>65</v>
       </c>
       <c r="E116">
@@ -2400,7 +2404,7 @@
       <c r="C117">
         <v>19</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="1">
         <v>65</v>
       </c>
       <c r="E117">
@@ -2417,7 +2421,7 @@
       <c r="C118">
         <v>63</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="1">
         <v>65</v>
       </c>
       <c r="E118">
@@ -2434,7 +2438,7 @@
       <c r="C119">
         <v>49</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="1">
         <v>65</v>
       </c>
       <c r="E119">
@@ -2451,7 +2455,7 @@
       <c r="C120">
         <v>51</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="1">
         <v>67</v>
       </c>
       <c r="E120">
@@ -2468,7 +2472,7 @@
       <c r="C121">
         <v>50</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="1">
         <v>67</v>
       </c>
       <c r="E121">
@@ -2485,7 +2489,7 @@
       <c r="C122">
         <v>27</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="1">
         <v>67</v>
       </c>
       <c r="E122">
@@ -2502,7 +2506,7 @@
       <c r="C123">
         <v>38</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="1">
         <v>67</v>
       </c>
       <c r="E123">
@@ -2519,7 +2523,7 @@
       <c r="C124">
         <v>40</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="1">
         <v>69</v>
       </c>
       <c r="E124">
@@ -2536,7 +2540,7 @@
       <c r="C125">
         <v>39</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="1">
         <v>69</v>
       </c>
       <c r="E125">
@@ -2553,7 +2557,7 @@
       <c r="C126">
         <v>23</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="1">
         <v>70</v>
       </c>
       <c r="E126">
@@ -2570,7 +2574,7 @@
       <c r="C127">
         <v>31</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="1">
         <v>70</v>
       </c>
       <c r="E127">
@@ -2587,7 +2591,7 @@
       <c r="C128">
         <v>43</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="1">
         <v>71</v>
       </c>
       <c r="E128">
@@ -2604,7 +2608,7 @@
       <c r="C129">
         <v>40</v>
       </c>
-      <c r="D129">
+      <c r="D129" s="1">
         <v>71</v>
       </c>
       <c r="E129">
@@ -2621,7 +2625,7 @@
       <c r="C130">
         <v>59</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="1">
         <v>71</v>
       </c>
       <c r="E130">
@@ -2638,7 +2642,7 @@
       <c r="C131">
         <v>38</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="1">
         <v>71</v>
       </c>
       <c r="E131">
@@ -2655,7 +2659,7 @@
       <c r="C132">
         <v>47</v>
       </c>
-      <c r="D132">
+      <c r="D132" s="1">
         <v>71</v>
       </c>
       <c r="E132">
@@ -2672,7 +2676,7 @@
       <c r="C133">
         <v>39</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="1">
         <v>71</v>
       </c>
       <c r="E133">
@@ -2689,7 +2693,7 @@
       <c r="C134">
         <v>25</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="1">
         <v>72</v>
       </c>
       <c r="E134">
@@ -2706,7 +2710,7 @@
       <c r="C135">
         <v>31</v>
       </c>
-      <c r="D135">
+      <c r="D135" s="1">
         <v>72</v>
       </c>
       <c r="E135">
@@ -2723,7 +2727,7 @@
       <c r="C136">
         <v>20</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="1">
         <v>73</v>
       </c>
       <c r="E136">
@@ -2740,7 +2744,7 @@
       <c r="C137">
         <v>29</v>
       </c>
-      <c r="D137">
+      <c r="D137" s="1">
         <v>73</v>
       </c>
       <c r="E137">
@@ -2757,7 +2761,7 @@
       <c r="C138">
         <v>44</v>
       </c>
-      <c r="D138">
+      <c r="D138" s="1">
         <v>73</v>
       </c>
       <c r="E138">
@@ -2774,7 +2778,7 @@
       <c r="C139">
         <v>32</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="1">
         <v>73</v>
       </c>
       <c r="E139">
@@ -2791,7 +2795,7 @@
       <c r="C140">
         <v>19</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="1">
         <v>74</v>
       </c>
       <c r="E140">
@@ -2808,7 +2812,7 @@
       <c r="C141">
         <v>35</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="1">
         <v>74</v>
       </c>
       <c r="E141">
@@ -2825,7 +2829,7 @@
       <c r="C142">
         <v>57</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="1">
         <v>75</v>
       </c>
       <c r="E142">
@@ -2842,7 +2846,7 @@
       <c r="C143">
         <v>32</v>
       </c>
-      <c r="D143">
+      <c r="D143" s="1">
         <v>75</v>
       </c>
       <c r="E143">
@@ -2859,7 +2863,7 @@
       <c r="C144">
         <v>28</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="1">
         <v>76</v>
       </c>
       <c r="E144">
@@ -2876,7 +2880,7 @@
       <c r="C145">
         <v>32</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="1">
         <v>76</v>
       </c>
       <c r="E145">
@@ -2893,7 +2897,7 @@
       <c r="C146">
         <v>25</v>
       </c>
-      <c r="D146">
+      <c r="D146" s="1">
         <v>77</v>
       </c>
       <c r="E146">
@@ -2910,7 +2914,7 @@
       <c r="C147">
         <v>28</v>
       </c>
-      <c r="D147">
+      <c r="D147" s="1">
         <v>77</v>
       </c>
       <c r="E147">
@@ -2927,7 +2931,7 @@
       <c r="C148">
         <v>48</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="1">
         <v>77</v>
       </c>
       <c r="E148">
@@ -2944,7 +2948,7 @@
       <c r="C149">
         <v>32</v>
       </c>
-      <c r="D149">
+      <c r="D149" s="1">
         <v>77</v>
       </c>
       <c r="E149">
@@ -2961,7 +2965,7 @@
       <c r="C150">
         <v>34</v>
       </c>
-      <c r="D150">
+      <c r="D150" s="1">
         <v>78</v>
       </c>
       <c r="E150">
@@ -2978,7 +2982,7 @@
       <c r="C151">
         <v>34</v>
       </c>
-      <c r="D151">
+      <c r="D151" s="1">
         <v>78</v>
       </c>
       <c r="E151">
@@ -2995,7 +2999,7 @@
       <c r="C152">
         <v>43</v>
       </c>
-      <c r="D152">
+      <c r="D152" s="1">
         <v>78</v>
       </c>
       <c r="E152">
@@ -3012,7 +3016,7 @@
       <c r="C153">
         <v>39</v>
       </c>
-      <c r="D153">
+      <c r="D153" s="1">
         <v>78</v>
       </c>
       <c r="E153">
@@ -3029,7 +3033,7 @@
       <c r="C154">
         <v>44</v>
       </c>
-      <c r="D154">
+      <c r="D154" s="1">
         <v>78</v>
       </c>
       <c r="E154">
@@ -3046,7 +3050,7 @@
       <c r="C155">
         <v>38</v>
       </c>
-      <c r="D155">
+      <c r="D155" s="1">
         <v>78</v>
       </c>
       <c r="E155">
@@ -3063,7 +3067,7 @@
       <c r="C156">
         <v>47</v>
       </c>
-      <c r="D156">
+      <c r="D156" s="1">
         <v>78</v>
       </c>
       <c r="E156">
@@ -3080,7 +3084,7 @@
       <c r="C157">
         <v>27</v>
       </c>
-      <c r="D157">
+      <c r="D157" s="1">
         <v>78</v>
       </c>
       <c r="E157">
@@ -3097,7 +3101,7 @@
       <c r="C158">
         <v>37</v>
       </c>
-      <c r="D158">
+      <c r="D158" s="1">
         <v>78</v>
       </c>
       <c r="E158">
@@ -3114,7 +3118,7 @@
       <c r="C159">
         <v>30</v>
       </c>
-      <c r="D159">
+      <c r="D159" s="1">
         <v>78</v>
       </c>
       <c r="E159">
@@ -3131,7 +3135,7 @@
       <c r="C160">
         <v>34</v>
       </c>
-      <c r="D160">
+      <c r="D160" s="1">
         <v>78</v>
       </c>
       <c r="E160">
@@ -3148,7 +3152,7 @@
       <c r="C161">
         <v>30</v>
       </c>
-      <c r="D161">
+      <c r="D161" s="1">
         <v>78</v>
       </c>
       <c r="E161">
@@ -3165,7 +3169,7 @@
       <c r="C162">
         <v>56</v>
       </c>
-      <c r="D162">
+      <c r="D162" s="1">
         <v>79</v>
       </c>
       <c r="E162">
@@ -3182,7 +3186,7 @@
       <c r="C163">
         <v>29</v>
       </c>
-      <c r="D163">
+      <c r="D163" s="1">
         <v>79</v>
       </c>
       <c r="E163">
@@ -3199,7 +3203,7 @@
       <c r="C164">
         <v>19</v>
       </c>
-      <c r="D164">
+      <c r="D164" s="1">
         <v>81</v>
       </c>
       <c r="E164">
@@ -3216,7 +3220,7 @@
       <c r="C165">
         <v>31</v>
       </c>
-      <c r="D165">
+      <c r="D165" s="1">
         <v>81</v>
       </c>
       <c r="E165">
@@ -3233,7 +3237,7 @@
       <c r="C166">
         <v>50</v>
       </c>
-      <c r="D166">
+      <c r="D166" s="1">
         <v>85</v>
       </c>
       <c r="E166">
@@ -3250,7 +3254,7 @@
       <c r="C167">
         <v>36</v>
       </c>
-      <c r="D167">
+      <c r="D167" s="1">
         <v>85</v>
       </c>
       <c r="E167">
@@ -3267,7 +3271,7 @@
       <c r="C168">
         <v>42</v>
       </c>
-      <c r="D168">
+      <c r="D168" s="1">
         <v>86</v>
       </c>
       <c r="E168">
@@ -3284,7 +3288,7 @@
       <c r="C169">
         <v>33</v>
       </c>
-      <c r="D169">
+      <c r="D169" s="1">
         <v>86</v>
       </c>
       <c r="E169">
@@ -3301,7 +3305,7 @@
       <c r="C170">
         <v>36</v>
       </c>
-      <c r="D170">
+      <c r="D170" s="1">
         <v>87</v>
       </c>
       <c r="E170">
@@ -3318,7 +3322,7 @@
       <c r="C171">
         <v>32</v>
       </c>
-      <c r="D171">
+      <c r="D171" s="1">
         <v>87</v>
       </c>
       <c r="E171">
@@ -3335,7 +3339,7 @@
       <c r="C172">
         <v>40</v>
       </c>
-      <c r="D172">
+      <c r="D172" s="1">
         <v>87</v>
       </c>
       <c r="E172">
@@ -3352,7 +3356,7 @@
       <c r="C173">
         <v>28</v>
       </c>
-      <c r="D173">
+      <c r="D173" s="1">
         <v>87</v>
       </c>
       <c r="E173">
@@ -3369,7 +3373,7 @@
       <c r="C174">
         <v>36</v>
       </c>
-      <c r="D174">
+      <c r="D174" s="1">
         <v>87</v>
       </c>
       <c r="E174">
@@ -3386,7 +3390,7 @@
       <c r="C175">
         <v>36</v>
       </c>
-      <c r="D175">
+      <c r="D175" s="1">
         <v>87</v>
       </c>
       <c r="E175">
@@ -3403,7 +3407,7 @@
       <c r="C176">
         <v>52</v>
       </c>
-      <c r="D176">
+      <c r="D176" s="1">
         <v>88</v>
       </c>
       <c r="E176">
@@ -3420,7 +3424,7 @@
       <c r="C177">
         <v>30</v>
       </c>
-      <c r="D177">
+      <c r="D177" s="1">
         <v>88</v>
       </c>
       <c r="E177">
@@ -3437,7 +3441,7 @@
       <c r="C178">
         <v>58</v>
       </c>
-      <c r="D178">
+      <c r="D178" s="1">
         <v>88</v>
       </c>
       <c r="E178">
@@ -3454,7 +3458,7 @@
       <c r="C179">
         <v>27</v>
       </c>
-      <c r="D179">
+      <c r="D179" s="1">
         <v>88</v>
       </c>
       <c r="E179">
@@ -3471,7 +3475,7 @@
       <c r="C180">
         <v>59</v>
       </c>
-      <c r="D180">
+      <c r="D180" s="1">
         <v>93</v>
       </c>
       <c r="E180">
@@ -3488,7 +3492,7 @@
       <c r="C181">
         <v>35</v>
       </c>
-      <c r="D181">
+      <c r="D181" s="1">
         <v>93</v>
       </c>
       <c r="E181">
@@ -3505,7 +3509,7 @@
       <c r="C182">
         <v>37</v>
       </c>
-      <c r="D182">
+      <c r="D182" s="1">
         <v>97</v>
       </c>
       <c r="E182">
@@ -3522,7 +3526,7 @@
       <c r="C183">
         <v>32</v>
       </c>
-      <c r="D183">
+      <c r="D183" s="1">
         <v>97</v>
       </c>
       <c r="E183">
@@ -3539,7 +3543,7 @@
       <c r="C184">
         <v>46</v>
       </c>
-      <c r="D184">
+      <c r="D184" s="1">
         <v>98</v>
       </c>
       <c r="E184">
@@ -3556,7 +3560,7 @@
       <c r="C185">
         <v>29</v>
       </c>
-      <c r="D185">
+      <c r="D185" s="1">
         <v>98</v>
       </c>
       <c r="E185">
@@ -3573,7 +3577,7 @@
       <c r="C186">
         <v>41</v>
       </c>
-      <c r="D186">
+      <c r="D186" s="1">
         <v>99</v>
       </c>
       <c r="E186">
@@ -3590,7 +3594,7 @@
       <c r="C187">
         <v>30</v>
       </c>
-      <c r="D187">
+      <c r="D187" s="1">
         <v>99</v>
       </c>
       <c r="E187">
@@ -3607,7 +3611,7 @@
       <c r="C188">
         <v>54</v>
       </c>
-      <c r="D188">
+      <c r="D188" s="1">
         <v>101</v>
       </c>
       <c r="E188">
@@ -3624,7 +3628,7 @@
       <c r="C189">
         <v>28</v>
       </c>
-      <c r="D189">
+      <c r="D189" s="1">
         <v>101</v>
       </c>
       <c r="E189">
@@ -3641,7 +3645,7 @@
       <c r="C190">
         <v>41</v>
       </c>
-      <c r="D190">
+      <c r="D190" s="1">
         <v>103</v>
       </c>
       <c r="E190">
@@ -3658,7 +3662,7 @@
       <c r="C191">
         <v>36</v>
       </c>
-      <c r="D191">
+      <c r="D191" s="1">
         <v>103</v>
       </c>
       <c r="E191">
@@ -3675,7 +3679,7 @@
       <c r="C192">
         <v>34</v>
       </c>
-      <c r="D192">
+      <c r="D192" s="1">
         <v>103</v>
       </c>
       <c r="E192">
@@ -3692,7 +3696,7 @@
       <c r="C193">
         <v>32</v>
       </c>
-      <c r="D193">
+      <c r="D193" s="1">
         <v>103</v>
       </c>
       <c r="E193">
@@ -3709,7 +3713,7 @@
       <c r="C194">
         <v>33</v>
       </c>
-      <c r="D194">
+      <c r="D194" s="1">
         <v>113</v>
       </c>
       <c r="E194">
@@ -3726,7 +3730,7 @@
       <c r="C195">
         <v>38</v>
       </c>
-      <c r="D195">
+      <c r="D195" s="1">
         <v>113</v>
       </c>
       <c r="E195">
@@ -3743,7 +3747,7 @@
       <c r="C196">
         <v>47</v>
       </c>
-      <c r="D196">
+      <c r="D196" s="1">
         <v>120</v>
       </c>
       <c r="E196">
@@ -3760,7 +3764,7 @@
       <c r="C197">
         <v>35</v>
       </c>
-      <c r="D197">
+      <c r="D197" s="1">
         <v>120</v>
       </c>
       <c r="E197">
@@ -3777,7 +3781,7 @@
       <c r="C198">
         <v>45</v>
       </c>
-      <c r="D198">
+      <c r="D198" s="1">
         <v>126</v>
       </c>
       <c r="E198">
@@ -3794,7 +3798,7 @@
       <c r="C199">
         <v>32</v>
       </c>
-      <c r="D199">
+      <c r="D199" s="1">
         <v>126</v>
       </c>
       <c r="E199">
@@ -3811,7 +3815,7 @@
       <c r="C200">
         <v>32</v>
       </c>
-      <c r="D200">
+      <c r="D200" s="1">
         <v>137</v>
       </c>
       <c r="E200">
@@ -3828,7 +3832,7 @@
       <c r="C201">
         <v>30</v>
       </c>
-      <c r="D201">
+      <c r="D201" s="1">
         <v>137</v>
       </c>
       <c r="E201">
@@ -3837,5 +3841,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>